<commit_message>
Nowe wykresy używające pakietu ggplot2
</commit_message>
<xml_diff>
--- a/Data_F.xlsx
+++ b/Data_F.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48533\Desktop\Prognozy-Lo-Piano-main\LoPIANO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markoni\Desktop\R\Pianino\Prognozy-Lo-Piano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FC5FFD-E677-4E27-890D-45FEEFF643D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3955F3-23B2-423A-AF37-81B74A03EC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -991,7 +991,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normalny 4" xfId="1" xr:uid="{274F8505-0F36-4533-9154-FAB0E4F71702}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -10093,7 +10093,7 @@
   <dimension ref="A1:L242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>